<commit_message>
connect the seperated line with trafo
</commit_message>
<xml_diff>
--- a/examples/create_scenario_with_grid/scenario_with_grid/electricity.xlsx
+++ b/examples/create_scenario_with_grid/scenario_with_grid/electricity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chujiahe/PycharmProjects/HAMLET/examples/create_scenario_with_grid/scenario_with_grid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F72DFFF-BE5C-664B-AE9B-5230E5C56C8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10328741-3CAC-EC4F-BA3E-3D0284F81417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="640" windowWidth="21060" windowHeight="17380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="640" windowWidth="21060" windowHeight="17380" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bus" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1343" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1347" uniqueCount="506">
   <si>
     <t>name</t>
   </si>
@@ -1955,8 +1955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17036,10 +17036,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:X19"/>
+  <dimension ref="A1:X20"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22:M89"/>
+    <sheetView tabSelected="1" zoomScale="185" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18390,6 +18390,77 @@
         <v>13</v>
       </c>
       <c r="X19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>33965</v>
+      </c>
+      <c r="B20" t="s">
+        <v>120</v>
+      </c>
+      <c r="C20" t="s">
+        <v>119</v>
+      </c>
+      <c r="D20">
+        <v>21819</v>
+      </c>
+      <c r="E20">
+        <v>29590</v>
+      </c>
+      <c r="F20">
+        <v>4.9999998882409996E-3</v>
+      </c>
+      <c r="G20">
+        <v>0.20669999718666099</v>
+      </c>
+      <c r="H20">
+        <v>8.0424778163433006E-2</v>
+      </c>
+      <c r="I20">
+        <v>829.99998331069946</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0.270000010728836</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20" t="s">
+        <v>97</v>
+      </c>
+      <c r="O20" t="b">
+        <v>1</v>
+      </c>
+      <c r="P20">
+        <v>0.82669997215270996</v>
+      </c>
+      <c r="Q20">
+        <v>0.32169911265373202</v>
+      </c>
+      <c r="R20">
+        <v>385.89999079704279</v>
+      </c>
+      <c r="S20">
+        <v>4.0299999527629998E-3</v>
+      </c>
+      <c r="T20">
+        <v>70</v>
+      </c>
+      <c r="V20">
+        <v>32153</v>
+      </c>
+      <c r="W20" t="s">
+        <v>13</v>
+      </c>
+      <c r="X20">
         <v>0</v>
       </c>
     </row>

</xml_diff>